<commit_message>
Update SRS review sheet: - Add points 8,9 ad 10 - Close points 2,3,5,6 and 7 Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specifications/SRS/Review.xlsx
+++ b/Software Specifications/SRS/Review.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
   <si>
     <t>Review point</t>
   </si>
@@ -57,6 +57,34 @@
   <si>
     <t>Please provide a reference table to have "Doc. No,
 Ref. Doc. Name, Ref. doc. Status".</t>
+  </si>
+  <si>
+    <t>13/2/2020</t>
+  </si>
+  <si>
+    <t>From requirement SRS_003 till SRS_010:
+Under which conditions this sequence will be applied you should declare that this requirement is valid if it's mode 1 , shall the developer implement this requirement without knowing the condition to apply this animation or this animation will be applied without any entry condition!
+The CYRS requirement is clear and saying that if the switch is high SW shall apply mode 1. please make the requirement clear how these requirements has not input !!! the input indeed is mode value (mode 1 or mode 2). 
+Also all these requirements shall be combined in one requirement as they represet the implementation of startup animation mode 1</t>
+  </si>
+  <si>
+    <t>Requirement SRS_011:
+Under which conditions this sequence will be applied you should declare that this requirement is valid if it's mode 2.</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Mali 13/2/2020: Point is closed</t>
+  </si>
+  <si>
+    <t>Mali 13/2/2020: Point still open</t>
+  </si>
+  <si>
+    <t>Remove status and history from the first page, first page shall be the cover for the doc.</t>
   </si>
 </sst>
 </file>
@@ -127,283 +155,589 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
+  <dxfs count="78">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
       </font>
     </dxf>
     <dxf>
@@ -771,16 +1105,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41.28515625" bestFit="1" customWidth="1"/>
@@ -816,13 +1150,17 @@
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="30">
+    <row r="3" spans="1:6">
       <c r="A3" s="7">
         <v>43984</v>
       </c>
@@ -832,11 +1170,15 @@
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="30">
       <c r="A4" s="7">
@@ -851,6 +1193,9 @@
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F4" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1">
       <c r="A5" s="7">
@@ -862,8 +1207,14 @@
       <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="D5" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1">
@@ -876,8 +1227,14 @@
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="D6" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="E6" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" ht="30">
@@ -890,102 +1247,334 @@
       <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D7" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="180">
+      <c r="A8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1">
-      <c r="A8" s="7"/>
-      <c r="C8" s="3"/>
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="45">
+      <c r="A9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="30">
+      <c r="A10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="containsText" dxfId="41" priority="20" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="77" priority="70" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="21" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="76" priority="71" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="22" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="75" priority="72" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="38" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="68" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="69" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E4">
-    <cfRule type="containsText" dxfId="36" priority="15" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="72" priority="65" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="16" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="71" priority="66" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="17" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="70" priority="67" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="30" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="63" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="64" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="23" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="67" priority="60" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="11" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="66" priority="61" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="12" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="65" priority="62" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="64" priority="57" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="63" priority="58" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="62" priority="59" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
+    <cfRule type="containsText" dxfId="61" priority="54" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="55" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="59" priority="56" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="containsText" dxfId="58" priority="51" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="52" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="56" priority="53" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="containsText" dxfId="55" priority="48" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="49" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="50" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="52" priority="45" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="51" priority="46" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="47" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="49" priority="42" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="43" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="44" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="containsText" dxfId="46" priority="39" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="40" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="41" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="cellIs" dxfId="43" priority="37" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="38" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="containsText" dxfId="41" priority="34" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="35" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="36" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="cellIs" dxfId="38" priority="32" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="33" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="containsText" dxfId="36" priority="29" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="30" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="31" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5">
+    <cfRule type="cellIs" dxfId="33" priority="27" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="containsText" dxfId="31" priority="24" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="25" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="26" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="28" priority="22" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="containsText" dxfId="26" priority="19" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="containsText" dxfId="21" priority="14" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="10" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
     <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3 D5:D7">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated SRS sheet based on review. Put document status and history in anew page and updating requiremnts tables addig input signals (mode selection signal) to the srs funcs (3->11)
</commit_message>
<xml_diff>
--- a/Software Specifications/SRS/Review.xlsx
+++ b/Software Specifications/SRS/Review.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
   <si>
     <t>Review point</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Acceptance</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>Remove Team names (under project name)</t>
@@ -90,8 +87,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,55 +152,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="78">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="72">
     <dxf>
       <font>
         <condense val="0"/>
@@ -863,7 +812,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -895,9 +844,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -929,6 +879,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1104,14 +1055,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63.42578125" customWidth="1"/>
@@ -1120,7 +1071,7 @@
     <col min="6" max="6" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1140,7 +1091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>43984</v>
       </c>
@@ -1148,19 +1099,19 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>43984</v>
       </c>
@@ -1168,19 +1119,19 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="30">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>43984</v>
       </c>
@@ -1188,16 +1139,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1">
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>43984</v>
       </c>
@@ -1205,19 +1156,19 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1">
+    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>43984</v>
       </c>
@@ -1225,19 +1176,19 @@
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="30">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>43984</v>
       </c>
@@ -1245,328 +1196,328 @@
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="180">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="45">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="30">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="containsText" dxfId="77" priority="70" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="71" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="72" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="69" priority="72" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="74" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="68" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="69" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E4">
-    <cfRule type="containsText" dxfId="72" priority="65" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="66" priority="65" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="66" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="65" priority="66" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="67" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="64" priority="67" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="69" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="63" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="67" priority="60" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="61" priority="60" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="61" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="60" priority="61" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="62" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="59" priority="62" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="64" priority="57" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="58" priority="57" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="58" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="57" priority="58" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="59" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="56" priority="59" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="61" priority="54" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="55" priority="54" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="55" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="56" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="53" priority="56" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="58" priority="51" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="52" priority="51" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="52" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="51" priority="52" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="53" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="50" priority="53" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="55" priority="48" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="49" priority="48" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="49" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="50" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="47" priority="50" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="52" priority="45" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="46" priority="45" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="46" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="45" priority="46" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="47" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="44" priority="47" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="49" priority="42" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="43" priority="42" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="43" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="42" priority="43" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="44" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="41" priority="44" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="containsText" dxfId="46" priority="39" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="40" priority="39" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="40" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="39" priority="40" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="41" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="38" priority="41" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="43" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="41" priority="34" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="35" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="36" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="38" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="36" priority="29" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="30" priority="29" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="30" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="29" priority="30" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="31" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="28" priority="31" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="33" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="31" priority="24" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="25" priority="24" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="25" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="26" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="23" priority="26" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="28" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="26" priority="19" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="21" priority="14" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="10" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update points 4,8,9,10 and 11 Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specifications/SRS/Review.xlsx
+++ b/Software Specifications/SRS/Review.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
   <si>
     <t>Review point</t>
   </si>
@@ -65,30 +65,44 @@
 Also all these requirements shall be combined in one requirement as they represet the implementation of startup animation mode 1</t>
   </si>
   <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Mali 13/2/2020: Point is closed</t>
+  </si>
+  <si>
+    <t>Remove status and history from the first page, first page shall be the cover for the doc.</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
     <t>Requirement SRS_011:
-Under which conditions this sequence will be applied you should declare that this requirement is valid if it's mode 2.</t>
-  </si>
-  <si>
-    <t>Accepted</t>
-  </si>
-  <si>
-    <t>Closed</t>
-  </si>
-  <si>
-    <t>Mali 13/2/2020: Point is closed</t>
-  </si>
-  <si>
-    <t>Mali 13/2/2020: Point still open</t>
-  </si>
-  <si>
-    <t>Remove status and history from the first page, first page shall be the cover for the doc.</t>
+Under which conditions this sequence will be applied you should declare that this requirement is valid if it's mode 2.
+Also the requirement shall declare that the animation scenario is repeated two times.</t>
+  </si>
+  <si>
+    <t>Mali 19/2/2020: Point still open, as I said all requirements from 003 till 010 shall be combined you can't close the point by your self the reviewer shall take this decision not you,you can just accept or reject it</t>
+  </si>
+  <si>
+    <t>Mali 13/2/2020: Point still open
+Mali 19/2/2020: Point is closed</t>
+  </si>
+  <si>
+    <t>19/2/2020</t>
+  </si>
+  <si>
+    <t>Plea presentationse provide a context diagram as declared in the presentation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,7 +166,483 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="72">
+  <dxfs count="124">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -812,7 +1302,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -844,10 +1334,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -879,7 +1368,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1055,14 +1543,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63.42578125" customWidth="1"/>
@@ -1071,7 +1559,7 @@
     <col min="6" max="6" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1091,7 +1579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="7">
         <v>43984</v>
       </c>
@@ -1102,16 +1590,16 @@
         <v>7</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="7">
         <v>43984</v>
       </c>
@@ -1122,16 +1610,16 @@
         <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="30">
       <c r="A4" s="7">
         <v>43984</v>
       </c>
@@ -1141,14 +1629,17 @@
       <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D4" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="1" customFormat="1">
       <c r="A5" s="7">
         <v>43984</v>
       </c>
@@ -1159,16 +1650,16 @@
         <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="1" customFormat="1">
       <c r="A6" s="7">
         <v>43984</v>
       </c>
@@ -1179,16 +1670,16 @@
         <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="30">
       <c r="A7" s="7">
         <v>43984</v>
       </c>
@@ -1199,16 +1690,16 @@
         <v>11</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="180">
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
@@ -1218,11 +1709,15 @@
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="D8" s="6"/>
       <c r="E8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="75">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -1230,13 +1725,14 @@
         <v>3</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>15</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D9" s="6"/>
       <c r="E9" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="30">
       <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
@@ -1244,288 +1740,412 @@
         <v>3</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="30">
+      <c r="A11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="123" priority="96" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="122" priority="97" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="72" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="121" priority="98" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="68" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="94" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="95" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E4">
-    <cfRule type="containsText" dxfId="66" priority="65" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="118" priority="91" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="66" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="117" priority="92" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="67" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="116" priority="93" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="63" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="89" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="90" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="61" priority="60" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="113" priority="86" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="61" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="112" priority="87" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="62" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="111" priority="88" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="58" priority="57" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="110" priority="83" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="58" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="109" priority="84" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="59" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="108" priority="85" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="55" priority="54" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="107" priority="80" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="106" priority="81" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="56" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="105" priority="82" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="52" priority="51" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="104" priority="77" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="52" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="103" priority="78" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="53" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="102" priority="79" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="49" priority="48" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="101" priority="74" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="100" priority="75" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="50" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="99" priority="76" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="46" priority="45" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="98" priority="71" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="46" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="97" priority="72" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="47" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="96" priority="73" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="43" priority="42" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="95" priority="68" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="43" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="94" priority="69" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="44" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="93" priority="70" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="containsText" dxfId="40" priority="39" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="92" priority="65" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="40" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="91" priority="66" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="41" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="90" priority="67" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="63" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="64" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="87" priority="60" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="86" priority="61" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="85" priority="62" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="58" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="59" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="30" priority="29" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="82" priority="55" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="30" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="81" priority="56" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="31" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="80" priority="57" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="53" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="54" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="25" priority="24" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="77" priority="50" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="76" priority="51" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="26" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="75" priority="52" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="48" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="49" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="72" priority="45" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="71" priority="46" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="70" priority="47" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="43" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="44" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="67" priority="40" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="66" priority="41" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="65" priority="42" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="38" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="39" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="62" priority="35" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="61" priority="36" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="60" priority="37" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="33" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="34" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="57" priority="30" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="56" priority="31" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="55" priority="32" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="54" priority="27" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="53" priority="28" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="52" priority="29" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="cellIs" dxfId="51" priority="25" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="26" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="24" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="cellIs" dxfId="43" priority="21" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="22" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="cellIs" dxfId="39" priority="19" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="20" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="35" priority="17" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="18" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="31" priority="15" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="14" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3 D5:D7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update points 8,9,12,13,14 and 15 Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specifications/SRS/Review.xlsx
+++ b/Software Specifications/SRS/Review.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="31">
   <si>
     <t>Review point</t>
   </si>
@@ -85,9 +85,6 @@
 Also the requirement shall declare that the animation scenario is repeated two times.</t>
   </si>
   <si>
-    <t>Mali 19/2/2020: Point still open, as I said all requirements from 003 till 010 shall be combined you can't close the point by your self the reviewer shall take this decision not you,you can just accept or reject it</t>
-  </si>
-  <si>
     <t>Mali 13/2/2020: Point still open
 Mali 19/2/2020: Point is closed</t>
   </si>
@@ -95,7 +92,32 @@
     <t>19/2/2020</t>
   </si>
   <si>
-    <t>Plea presentationse provide a context diagram as declared in the presentation</t>
+    <t>Please provide a context diagram as declared in the presentation</t>
+  </si>
+  <si>
+    <t>24/2/2020</t>
+  </si>
+  <si>
+    <t>Date field in doc. History shall be the same format for all cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Split the requirements to section, section for all TI reuirements, section for all Tail requirements and section for startup modes reuirements </t>
+  </si>
+  <si>
+    <t>There is no requirement to configure the HW pins according to HSI pin descreption</t>
+  </si>
+  <si>
+    <t>In Software context: 
+- The inputs and outputs in the requireemnts shall be the same as output signals in sotware context for ex: 
+in SRS_018 I shall see "Tail LEDs status" in the context instead it's not exist and all the rest signals like that 
+- For the input side the signal for ex: "Mode signal" is input to "input feature block" and output from it at the same time !</t>
+  </si>
+  <si>
+    <t>Mali 19/2/2020: Point still open, as I said all requirements from 003 till 010 shall be combined you can't close the point by your self the reviewer shall take this decision not you,you can just accept or reject it
+Mali 24/2/200: Point is closed</t>
+  </si>
+  <si>
+    <t>Mali 24/2/200: Point is closed</t>
   </si>
 </sst>
 </file>
@@ -166,329 +188,1047 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="124">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
+  <dxfs count="210">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
@@ -1544,14 +2284,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
@@ -1636,7 +2377,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1">
@@ -1709,12 +2450,14 @@
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1" ht="75">
@@ -1727,9 +2470,14 @@
       <c r="C9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" ht="30">
@@ -1752,318 +2500,600 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="30">
+    <row r="11" spans="1:6" s="1" customFormat="1">
       <c r="A11" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="1" customFormat="1">
+      <c r="A12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="45">
+      <c r="A13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="30">
+      <c r="A14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" s="1" customFormat="1" ht="105">
+      <c r="A15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2">
-    <cfRule type="containsText" dxfId="123" priority="96" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="209" priority="152" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="97" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="208" priority="153" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="98" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="207" priority="154" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="120" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="150" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="151" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E4">
-    <cfRule type="containsText" dxfId="118" priority="91" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="204" priority="147" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="92" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="203" priority="148" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="93" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="202" priority="149" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="115" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="145" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="146" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="113" priority="86" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="199" priority="142" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="87" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="198" priority="143" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="88" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="197" priority="144" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="110" priority="83" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="196" priority="139" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="84" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="195" priority="140" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="85" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="194" priority="141" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="107" priority="80" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="193" priority="136" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="81" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="192" priority="137" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="82" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="191" priority="138" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="104" priority="77" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="190" priority="133" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="78" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="189" priority="134" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="79" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="188" priority="135" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="containsText" dxfId="101" priority="74" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="187" priority="130" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="75" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="186" priority="131" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="76" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="185" priority="132" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="98" priority="71" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="184" priority="127" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="72" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="183" priority="128" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="73" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="182" priority="129" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="containsText" dxfId="95" priority="68" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="181" priority="124" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="69" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="180" priority="125" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="70" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="179" priority="126" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="containsText" dxfId="92" priority="65" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="178" priority="121" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="66" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="177" priority="122" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="67" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="176" priority="123" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="89" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="119" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="120" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="87" priority="60" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="173" priority="116" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="61" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="172" priority="117" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="62" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="171" priority="118" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="84" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="114" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="115" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="82" priority="55" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="168" priority="111" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="56" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="167" priority="112" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="57" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="166" priority="113" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="cellIs" dxfId="79" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="109" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="110" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="77" priority="50" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="163" priority="106" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="51" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="162" priority="107" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="52" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="161" priority="108" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="74" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="104" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="105" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="72" priority="45" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="158" priority="101" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="46" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="157" priority="102" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="47" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="156" priority="103" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="69" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="99" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="100" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="67" priority="40" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="153" priority="96" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="41" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="152" priority="97" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="42" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="151" priority="98" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="64" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="94" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="95" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="containsText" dxfId="62" priority="35" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="148" priority="91" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="36" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="147" priority="92" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="37" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="146" priority="93" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="59" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="89" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="90" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsText" dxfId="57" priority="30" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="143" priority="86" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="31" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="142" priority="87" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="32" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="141" priority="88" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="containsText" dxfId="54" priority="27" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="140" priority="83" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="28" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="139" priority="84" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="29" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="138" priority="85" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="51" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="81" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="82" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="79" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="80" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="43" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="77" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="78" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
+    <cfRule type="cellIs" dxfId="131" priority="75" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="76" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="129" priority="73" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="74" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="127" priority="71" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="72" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="cellIs" dxfId="125" priority="69" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="124" priority="70" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="cellIs" dxfId="123" priority="67" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="68" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="121" priority="64" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="120" priority="65" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="119" priority="66" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="containsText" dxfId="118" priority="61" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="117" priority="62" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="116" priority="63" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="115" priority="59" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="60" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="113" priority="57" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="58" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="containsText" dxfId="111" priority="54" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="110" priority="55" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="56" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="containsText" dxfId="105" priority="51" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="104" priority="52" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="103" priority="53" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="cellIs" dxfId="99" priority="49" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="50" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="cellIs" dxfId="95" priority="47" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="48" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="containsText" dxfId="91" priority="44" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="90" priority="45" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="89" priority="46" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="containsText" dxfId="85" priority="41" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="84" priority="42" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="83" priority="43" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="79" priority="39" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="40" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="75" priority="37" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="38" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="containsText" dxfId="71" priority="34" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="70" priority="35" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="69" priority="36" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="containsText" dxfId="65" priority="31" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="32" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E14)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="33" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="cellIs" dxfId="59" priority="29" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="30" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="cellIs" dxfId="55" priority="27" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="28" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="containsText" dxfId="51" priority="24" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="25" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="26" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="22" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="23" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
     <cfRule type="cellIs" dxfId="39" priority="19" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
@@ -2071,7 +3101,7 @@
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
+  <conditionalFormatting sqref="D15">
     <cfRule type="cellIs" dxfId="35" priority="17" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
@@ -2079,73 +3109,71 @@
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="31" priority="14" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="15" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="16" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="25" priority="11" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="12" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="31" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
-      <formula>"Accepted"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",E11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",E11)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
-      <formula>"Accepted"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"Accepted"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D15">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E15">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated SRS according to review
</commit_message>
<xml_diff>
--- a/Software Specifications/SRS/Review.xlsx
+++ b/Software Specifications/SRS/Review.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7232599D-A10E-4A30-9587-4F2F166D8BAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="HSI review" sheetId="5" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="31">
   <si>
     <t>Review point</t>
   </si>
@@ -108,23 +107,23 @@
     <t>There is no requirement to configure the HW pins according to HSI pin descreption</t>
   </si>
   <si>
+    <t>Mali 19/2/2020: Point still open, as I said all requirements from 003 till 010 shall be combined you can't close the point by your self the reviewer shall take this decision not you,you can just accept or reject it
+Mali 24/2/200: Point is closed</t>
+  </si>
+  <si>
+    <t>Mali 24/2/200: Point is closed</t>
+  </si>
+  <si>
     <t>In Software context: 
-- The inputs and outputs in the requireemnts shall be the same as output signals in sotware context for ex: 
+- The inputs and outputs in the requirements shall be the same as output signals in sotware context for ex: 
 in SRS_018 I shall see "Tail LEDs status" in the context instead it's not exist and all the rest signals like that 
 - For the input side the signal for ex: "Mode signal" is input to "input feature block" and output from it at the same time !</t>
-  </si>
-  <si>
-    <t>Mali 19/2/2020: Point still open, as I said all requirements from 003 till 010 shall be combined you can't close the point by your self the reviewer shall take this decision not you,you can just accept or reject it
-Mali 24/2/200: Point is closed</t>
-  </si>
-  <si>
-    <t>Mali 24/2/200: Point is closed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1598,23 +1597,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1650,23 +1632,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1842,11 +1807,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2016,7 +1981,7 @@
         <v>16</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -2036,7 +2001,7 @@
         <v>16</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2107,7 +2072,9 @@
       <c r="C13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="6"/>
+      <c r="D13" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>19</v>
       </c>
@@ -2139,9 +2106,11 @@
         <v>3</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="E15" s="1" t="s">
         <v>19</v>
       </c>
@@ -2733,10 +2702,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D15" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D15">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E15" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E15">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>